<commit_message>
copied separate parts from queries to one column or each idiom
</commit_message>
<xml_diff>
--- a/results/idiom_database_sprenger_with_queries.xlsx
+++ b/results/idiom_database_sprenger_with_queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\Studie informatiekunde\master\master project\project\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449AE7E4-A8BC-4512-ACE7-3A881C0E2502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E966AC70-AFE7-4222-A90A-E7B869E42DDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,15 +17,23 @@
     <sheet name="verbeterd" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">idiom_database!$A$1:$R$297</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">idiom_database!$A$1:$O$297</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">verbeterd!$A$1:$A$23</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="1119">
   <si>
     <t>Idiom</t>
   </si>
@@ -2616,9 +2624,6 @@
     <t>([lemma="trekken"][]?[lemma="aan"][lemma="de"][lemma="bel"])|([lemma="aan"][lemma="de"][lemma="bel"][lemma="trekken"])</t>
   </si>
   <si>
-    <t>Freq. Total</t>
-  </si>
-  <si>
     <t>([lemma = "kijken" ] [ lemma = "de" ] [ lemma = "kat" ] [ lemma= "uit" ] [ lemma= "de" ] [ lemma= "boom" ]) | ([lemma = "kijken" ] [] [ lemma = "de" ] [ lemma = "kat" ] [ lemma= "uit" ] [ lemma= "de" ] [ lemma= "boom" ])  | ([ lemma = "de" ] [ lemma = "kat" ] [ lemma= "uit" ] [ lemma= "de" ] [ lemma= "boom" ] [lemma="kijken"])</t>
   </si>
   <si>
@@ -3120,33 +3125,15 @@
     <t>([ lemma= "op" ] [ lemma= "de" ] [ lemma= "vuist" ])|</t>
   </si>
   <si>
-    <t>(([ lemma= "in" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "kaart" ] [ lemma= "spelen" ])|</t>
-  </si>
-  <si>
-    <t>([ lemma= "spelen" ] [  ]{1,2}[ lemma= "in" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "kaart" ]))|</t>
-  </si>
-  <si>
     <t>(([ lemma = "op" ] [ lemma = "zijn" ] [ pos_head = "adj" ]? [ word = "vestje" ] ([ lemma = "spugen" ]|[ lemma = "spuwen" ]))|(([ lemma = "spugen" ]|[ lemma = "spuwen" ])[ lemma = "op" ] [ lemma = "zijn" ] [ pos_head = "adj" ]? [ word = "vestje" ]))|</t>
   </si>
   <si>
-    <t>(([ lemma= "in" ] [] [ pos_head = "adj" ]? [ lemma= "hemd" ] [lemma="staan"])|</t>
-  </si>
-  <si>
-    <t>([lemma="staan"] []? [ lemma= "in" ] [] [ pos_head = "adj" ]? [ lemma= "hemd" ]))|</t>
-  </si>
-  <si>
     <t>([ lemma= "gat" ] [ lemma= "in" ] [] [ pos_head = "adj" ]? [ lemma= "hoofd" ])|</t>
   </si>
   <si>
     <t>([ lemma= "maas" ] [ lemma= "van" ] [ lemma= "het" ] [ pos_head = "adj" ]? [ lemma= "net" ])|</t>
   </si>
   <si>
-    <t>(([ lemma= "vallen" ] [  ]?[ lemma= "in" ] [ lemma= "een" ] [ pos_head = "adj" ]? [ lemma= "gat" ])|</t>
-  </si>
-  <si>
-    <t>([ lemma= "in" ] [ lemma= "een" ] [ pos_head = "adj" ]? [ lemma= "gat" ] [ lemma= "vallen" ]))|</t>
-  </si>
-  <si>
     <t>([ lemma= "in" ] [ lemma= "het" ] [ pos_head = "adj" ]? [ lemma= "achterhoofd" ])|</t>
   </si>
   <si>
@@ -3162,21 +3149,9 @@
     <t>([ lemma= "met" ] [ pos_head = "adj" ]? [ lemma= "vlag" ] [ lemma= "en" ] [ pos_head = "adj" ]? [ lemma= "wimpel" ])|</t>
   </si>
   <si>
-    <t>(([ lemma= "doen" ] [  ]?[ lemma= "van" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "hand" ])|</t>
-  </si>
-  <si>
-    <t>([ lemma= "van" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "hand" ] [ lemma= "doen" ]))|</t>
-  </si>
-  <si>
     <t>([ lemma= "het" ] [ lemma= "in" ] [ lemma= "zijn" ] [ pos_head = "adj" ]? [ lemma= "broek" ])|</t>
   </si>
   <si>
-    <t>(([ lemma= "uit" ] [ ] [ pos_head = "adj" ]? [ lemma= "hoofd" ] [lemma="leren"])|</t>
-  </si>
-  <si>
-    <t>([lemma="leren"] []{1,2} [ lemma= "uit" ] [ ] [ pos_head = "adj" ]? [ lemma= "hoofd" ] ))|</t>
-  </si>
-  <si>
     <t>(([ lemma= "onder" ] [] [ pos_head = "adj" ]? [ lemma= "pet" ][lemma="houden"]) | ([lemma="houden"] []{1,2}[ lemma= "onder" ] [] [ pos_head = "adj" ]? [ lemma= "pet" ]))|</t>
   </si>
   <si>
@@ -3192,30 +3167,12 @@
     <t>([ lemma= "achter" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "geranium" ])|</t>
   </si>
   <si>
-    <t>(([lemma="kloppen"][]?[ lemma= "zich" ] [ lemma= "op" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "borst" ])|</t>
-  </si>
-  <si>
-    <t>([ lemma= "op" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "borst" ][lemma="kloppen"]))|</t>
-  </si>
-  <si>
     <t>([ lemma= "op" ] [ lemma= "zijn" ] [ pos_head = "adj" ]? [ lemma= "ziel" ])|</t>
   </si>
   <si>
-    <t>(([lemma="toveren"][]?[lemma= "iets" ] [ lemma= "uit" ] [ ] [ pos_head = "adj" ]? [ lemma= "hoed" ])|</t>
-  </si>
-  <si>
-    <t>([ lemma= "iets" ] [ lemma= "uit" ] [  ] [ pos_head = "adj" ]? [ lemma= "hoed" ][lemma="toveren"]))|</t>
-  </si>
-  <si>
     <t>([ lemma= "bij" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "duivel" ] [ lemma= "te" ] [ lemma= "biecht" ])|</t>
   </si>
   <si>
-    <t>(([ lemma= "strijken" ] [  ]?[ lemma= "met" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "eer" ])|</t>
-  </si>
-  <si>
-    <t>([ lemma= "met" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "eer" ] [  ]?[ lemma= "strijken" ]))|</t>
-  </si>
-  <si>
     <t>([ lemma= "voor" ] [ lemma= "het" ] [ pos_head = "adj" ]? [ lemma= "voetlicht" ])|</t>
   </si>
   <si>
@@ -3246,12 +3203,6 @@
     <t>([ lemma= "op" ] [] [ pos_head = "adj" ]? [ word= "duimpje" ])|</t>
   </si>
   <si>
-    <t>(([lemma="zitten"][]?[lemma= "op" ] [ pos_head = "adj" ]? [ lemma= "rozen" ])|</t>
-  </si>
-  <si>
-    <t>([lemma= "op" ] [ pos_head = "adj" ]? [ lemma= "rozen" ][lemma="zitten"]))|</t>
-  </si>
-  <si>
     <t>(([ lemma= "in" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "arm" ] [lemma="nemen"])|([lemma="nemen"][]{1,3}[ lemma= "in" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "arm" ]))|</t>
   </si>
   <si>
@@ -3264,21 +3215,9 @@
     <t>(([lemma="helpen"] [pos_head = "vnw"] [ lemma= "op" ] []? [ pos_head = "adj" ]? [ lemma= "weg" ] )|([pos_head = "vnw"] [ lemma= "op" ] []? [ pos_head = "adj" ]? [ lemma= "weg" ] []? [lemma="helpen"]))|</t>
   </si>
   <si>
-    <t>(([lemma="draaien"][]{0,2}[word="duimen"])|</t>
-  </si>
-  <si>
-    <t>([lemma="duimen"][]?[lemma="draaien"]))|</t>
-  </si>
-  <si>
     <t>([ lemma= "leven" ] [ lemma= "in" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "brouwerij" ])|</t>
   </si>
   <si>
-    <t>(([ lemma= "houden" ] [  ]{1,2}[ lemma= "aan" ] [ lemma= "zijn" ] [ pos_head = "adj" ]? [ lemma= "woord" ])|</t>
-  </si>
-  <si>
-    <t>([ lemma= "aan" ] [ lemma= "zijn" ] [ pos_head = "adj" ]? [ lemma= "woord" ] [ lemma= "houden" ]))|</t>
-  </si>
-  <si>
     <t>([ lemma= "boel" ] [ lemma= "op" ] [ pos_head = "adj" ]? [ lemma= "stelt" ])|</t>
   </si>
   <si>
@@ -3354,12 +3293,6 @@
     <t>([ lemma= "op" ] [pos_head = "adj"]? [ lemma= "sleeptouw" ])|</t>
   </si>
   <si>
-    <t>(([lemma="roeien"][]?[ lemma= "tegen" ] [ lemma= "de" ] [pos_head = "adj"]? [ lemma= "stroom" ] [ lemma= "op" ])|</t>
-  </si>
-  <si>
-    <t>([ lemma= "tegen" ] [ lemma= "de" ] [pos_head = "adj"]? [ lemma= "stroom" ] [ lemma= "op" ][lemma="roeien"]))|</t>
-  </si>
-  <si>
     <t>([lemma = "lopen"] []? [ lemma= "in" ] [ lemma= "het" ] ([ lemma= "honderd" ]|[lemma="100"]))</t>
   </si>
   <si>
@@ -3381,27 +3314,9 @@
     <t>([ lemma= "deur" ] [ lemma= "op" ] [ lemma= "een" ] [pos_head = "adj"]? [ lemma= "kier" ])|</t>
   </si>
   <si>
-    <t>(([lemma="van"][pos_head = "vnw"][pos_head = "adj"]?[lemma="bed"][lemma="lichten"])|</t>
-  </si>
-  <si>
-    <t>([lemma="lichten"][]{0,2}[lemma="van"][pos_head = "vnw"][pos_head = "adj"]?[lemma="bed"]))|</t>
-  </si>
-  <si>
-    <t>(([lemma="trekken"][]?[lemma="aan"][lemma="de"][pos_head = "adj"]?[lemma="bel"])|</t>
-  </si>
-  <si>
-    <t>([lemma="aan"][lemma="de"][pos_head = "adj"]?[lemma="bel"][lemma="trekken"]))|</t>
-  </si>
-  <si>
     <t>([ lemma= "achter" ] [ lemma= "de" ] [pos_head = "adj"]? [ lemma= "hand" ])|</t>
   </si>
   <si>
-    <t>(([lemma="vechten"][]?[lemma="tegen"][pos_head = "adj"]?[lemma="windmolen"])|</t>
-  </si>
-  <si>
-    <t>([lemma="tegen"][pos_head = "adj"]?[lemma="windmolen"][lemma="vechten"]))|</t>
-  </si>
-  <si>
     <t>([ lemma= "voor" ] [ lemma= "zijn" ] [pos_head = "adj"]? [word = "kiezen" ])|</t>
   </si>
   <si>
@@ -3417,16 +3332,64 @@
     <t>(([lemma="zich"][ lemma = "in" ] ([ lemma = "de" ]|[pos_head="vnw"]) [ pos_head = "adj" ]? [ word = "vingers" ] [ lemma = "snijden" ])|([ lemma = "snijden" ][pos_head="vnw"]?[lemma="zich"][ lemma = "in" ] ([ lemma = "de" ]|[pos_head="vnw"]) [ pos_head = "adj" ]? [ word = "vingers" ]))|</t>
   </si>
   <si>
-    <t>(([ lemma= "op" ] [ lemma= "straat" ] [ lemma= "zetten" ])|</t>
-  </si>
-  <si>
-    <t>([ lemma= "zetten" ] [pos_head = "spec" | pos_head = "vnw"]{0,2}[ lemma= "op" ] []? [ lemma= "straat" ]))|</t>
-  </si>
-  <si>
     <t>([ lemma= "gesprek" ] [ lemma= "van" ] [ lemma= "de" ] [pos_head = "adj"]? [ lemma= "dag" ])</t>
   </si>
   <si>
     <t>([ lemma= "in" ] [ lemma= "de" ] [pos_head = "adj"]? [ word= "vingers" ])|</t>
+  </si>
+  <si>
+    <t>(([ lemma= "doen" ] [  ]?[ lemma= "van" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "hand" ])|([ lemma= "van" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "hand" ] [ lemma= "doen" ]))|</t>
+  </si>
+  <si>
+    <t>(([lemma="draaien"][]{0,2}[word="duimen"])|([lemma="duimen"][]?[lemma="draaien"]))|</t>
+  </si>
+  <si>
+    <t>(([ lemma= "houden" ] [  ]{1,2}[ lemma= "aan" ] [ lemma= "zijn" ] [ pos_head = "adj" ]? [ lemma= "woord" ])|([ lemma= "aan" ] [ lemma= "zijn" ] [ pos_head = "adj" ]? [ lemma= "woord" ] [ lemma= "houden" ]))|</t>
+  </si>
+  <si>
+    <t>(([lemma="kloppen"][]?[ lemma= "zich" ] [ lemma= "op" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "borst" ])|([ lemma= "op" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "borst" ][lemma="kloppen"]))|</t>
+  </si>
+  <si>
+    <t>(([ lemma= "uit" ] [ ] [ pos_head = "adj" ]? [ lemma= "hoofd" ] [lemma="leren"])|([lemma="leren"] []{1,2} [ lemma= "uit" ] [ ] [ pos_head = "adj" ]? [ lemma= "hoofd" ] ))|</t>
+  </si>
+  <si>
+    <t>(([lemma="van"][pos_head = "vnw"][pos_head = "adj"]?[lemma="bed"][lemma="lichten"])|([lemma="lichten"][]{0,2}[lemma="van"][pos_head = "vnw"][pos_head = "adj"]?[lemma="bed"]))|</t>
+  </si>
+  <si>
+    <t>(([lemma="roeien"][]?[ lemma= "tegen" ] [ lemma= "de" ] [pos_head = "adj"]? [ lemma= "stroom" ] [ lemma= "op" ])|([ lemma= "tegen" ] [ lemma= "de" ] [pos_head = "adj"]? [ lemma= "stroom" ] [ lemma= "op" ][lemma="roeien"]))|</t>
+  </si>
+  <si>
+    <t>(([ lemma= "in" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "kaart" ] [ lemma= "spelen" ])|([ lemma= "spelen" ] [  ]{1,2}[ lemma= "in" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "kaart" ]))|</t>
+  </si>
+  <si>
+    <t>(([ lemma= "in" ] [] [ pos_head = "adj" ]? [ lemma= "hemd" ] [lemma="staan"])|([lemma="staan"] []? [ lemma= "in" ] [] [ pos_head = "adj" ]? [ lemma= "hemd" ]))|</t>
+  </si>
+  <si>
+    <t>(([ lemma= "strijken" ] [  ]?[ lemma= "met" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "eer" ])|([ lemma= "met" ] [ lemma= "de" ] [ pos_head = "adj" ]? [ lemma= "eer" ] [  ]?[ lemma= "strijken" ]))|</t>
+  </si>
+  <si>
+    <t>(([lemma="toveren"][]?[lemma= "iets" ] [ lemma= "uit" ] [ ] [ pos_head = "adj" ]? [ lemma= "hoed" ])|([ lemma= "iets" ] [ lemma= "uit" ] [  ] [ pos_head = "adj" ]? [ lemma= "hoed" ][lemma="toveren"]))|</t>
+  </si>
+  <si>
+    <t>(([lemma="trekken"][]?[lemma="aan"][lemma="de"][pos_head = "adj"]?[lemma="bel"])|([lemma="aan"][lemma="de"][pos_head = "adj"]?[lemma="bel"][lemma="trekken"]))|</t>
+  </si>
+  <si>
+    <t>(([ lemma= "vallen" ] [  ]?[ lemma= "in" ] [ lemma= "een" ] [ pos_head = "adj" ]? [ lemma= "gat" ])|([ lemma= "in" ] [ lemma= "een" ] [ pos_head = "adj" ]? [ lemma= "gat" ] [ lemma= "vallen" ]))|</t>
+  </si>
+  <si>
+    <t>(([lemma="vechten"][]?[lemma="tegen"][pos_head = "adj"]?[lemma="windmolen"])|([lemma="tegen"][pos_head = "adj"]?[lemma="windmolen"][lemma="vechten"]))|</t>
+  </si>
+  <si>
+    <t>(([lemma="zitten"][]?[lemma= "op" ] [ pos_head = "adj" ]? [ lemma= "rozen" ])|([lemma= "op" ] [ pos_head = "adj" ]? [ lemma= "rozen" ][lemma="zitten"]))|</t>
+  </si>
+  <si>
+    <t>(([ lemma= "op" ] [ lemma= "straat" ] [ lemma= "zetten" ])|([ lemma= "zetten" ] [pos_head = "spec" | pos_head = "vnw"]{0,2}[ lemma= "op" ] []? [ lemma= "straat" ]))|</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Query</t>
   </si>
 </sst>
 </file>
@@ -4308,10 +4271,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R194"/>
+  <dimension ref="A1:P255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P115" sqref="P115"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4329,11 +4292,9 @@
     <col min="13" max="13" width="54.28515625" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="112.5703125" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="202.85546875" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="162.28515625" customWidth="1"/>
-    <col min="17" max="17" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4380,10 +4341,10 @@
         <v>738</v>
       </c>
       <c r="P1" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>260</v>
       </c>
@@ -4430,10 +4391,10 @@
         <v>786</v>
       </c>
       <c r="P2" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -4480,10 +4441,10 @@
         <v>767</v>
       </c>
       <c r="P3" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -4530,10 +4491,10 @@
         <v>761</v>
       </c>
       <c r="P4" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>271</v>
       </c>
@@ -4580,10 +4541,10 @@
         <v>788</v>
       </c>
       <c r="P5" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>683</v>
       </c>
@@ -4630,10 +4591,10 @@
         <v>844</v>
       </c>
       <c r="P6" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -4680,10 +4641,10 @@
         <v>750</v>
       </c>
       <c r="P7" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>584</v>
       </c>
@@ -4730,10 +4691,10 @@
         <v>831</v>
       </c>
       <c r="P8" t="s">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>454</v>
       </c>
@@ -4780,10 +4741,10 @@
         <v>814</v>
       </c>
       <c r="P9" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>572</v>
       </c>
@@ -4830,10 +4791,10 @@
         <v>829</v>
       </c>
       <c r="P10" t="s">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>317</v>
       </c>
@@ -4880,10 +4841,10 @@
         <v>796</v>
       </c>
       <c r="P11" t="s">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -4930,10 +4891,10 @@
         <v>742</v>
       </c>
       <c r="P12" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>466</v>
       </c>
@@ -4980,10 +4941,10 @@
         <v>816</v>
       </c>
       <c r="P13" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>462</v>
       </c>
@@ -5030,13 +4991,10 @@
         <v>858</v>
       </c>
       <c r="P14" t="s">
-        <v>1045</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -5083,10 +5041,10 @@
         <v>752</v>
       </c>
       <c r="P15" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>211</v>
       </c>
@@ -5133,10 +5091,10 @@
         <v>782</v>
       </c>
       <c r="P16" t="s">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>568</v>
       </c>
@@ -5183,13 +5141,10 @@
         <v>856</v>
       </c>
       <c r="P17" t="s">
-        <v>1079</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>310</v>
       </c>
@@ -5236,10 +5191,10 @@
         <v>795</v>
       </c>
       <c r="P18" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>504</v>
       </c>
@@ -5286,10 +5241,10 @@
         <v>821</v>
       </c>
       <c r="P19" t="s">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>614</v>
       </c>
@@ -5336,10 +5291,10 @@
         <v>836</v>
       </c>
       <c r="P20" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -5386,10 +5341,10 @@
         <v>753</v>
       </c>
       <c r="P21" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>409</v>
       </c>
@@ -5436,10 +5391,10 @@
         <v>810</v>
       </c>
       <c r="P22" t="s">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>437</v>
       </c>
@@ -5486,10 +5441,10 @@
         <v>811</v>
       </c>
       <c r="P23" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>125</v>
       </c>
@@ -5536,10 +5491,10 @@
         <v>764</v>
       </c>
       <c r="P24" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>561</v>
       </c>
@@ -5586,10 +5541,10 @@
         <v>828</v>
       </c>
       <c r="P25" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>146</v>
       </c>
@@ -5636,10 +5591,10 @@
         <v>766</v>
       </c>
       <c r="P26" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>245</v>
       </c>
@@ -5686,10 +5641,10 @@
         <v>785</v>
       </c>
       <c r="P27" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>91</v>
       </c>
@@ -5736,10 +5691,10 @@
         <v>756</v>
       </c>
       <c r="P28" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>388</v>
       </c>
@@ -5786,10 +5741,10 @@
         <v>807</v>
       </c>
       <c r="P29" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -5836,10 +5791,10 @@
         <v>749</v>
       </c>
       <c r="P30" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>527</v>
       </c>
@@ -5886,10 +5841,10 @@
         <v>826</v>
       </c>
       <c r="P31" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>543</v>
       </c>
@@ -5933,10 +5888,10 @@
         <v>545</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="P32" t="s">
-        <v>1071</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -5986,7 +5941,7 @@
         <v>805</v>
       </c>
       <c r="P33" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -6036,7 +5991,7 @@
         <v>817</v>
       </c>
       <c r="P34" t="s">
-        <v>1051</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -6086,7 +6041,7 @@
         <v>804</v>
       </c>
       <c r="P35" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -6133,10 +6088,10 @@
         <v>210</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="P36" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -6183,10 +6138,10 @@
         <v>641</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="P37" t="s">
-        <v>1099</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -6236,7 +6191,7 @@
         <v>787</v>
       </c>
       <c r="P38" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -6286,7 +6241,7 @@
         <v>746</v>
       </c>
       <c r="P39" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -6333,10 +6288,10 @@
         <v>436</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="P40" t="s">
-        <v>1036</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -6383,10 +6338,10 @@
         <v>141</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="P41" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -6436,7 +6391,7 @@
         <v>771</v>
       </c>
       <c r="P42" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -6486,7 +6441,7 @@
         <v>834</v>
       </c>
       <c r="P43" t="s">
-        <v>1091</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -6536,7 +6491,7 @@
         <v>777</v>
       </c>
       <c r="P44" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -6586,7 +6541,7 @@
         <v>802</v>
       </c>
       <c r="P45" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -6636,7 +6591,7 @@
         <v>853</v>
       </c>
       <c r="P46" t="s">
-        <v>1126</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -6686,7 +6641,7 @@
         <v>806</v>
       </c>
       <c r="P47" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -6733,13 +6688,13 @@
         <v>637</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="P48" t="s">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>397</v>
       </c>
@@ -6786,10 +6741,10 @@
         <v>808</v>
       </c>
       <c r="P49" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>711</v>
       </c>
@@ -6836,10 +6791,10 @@
         <v>850</v>
       </c>
       <c r="P50" t="s">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>655</v>
       </c>
@@ -6886,10 +6841,10 @@
         <v>840</v>
       </c>
       <c r="P51" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>294</v>
       </c>
@@ -6933,13 +6888,13 @@
         <v>297</v>
       </c>
       <c r="O52" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="P52" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>175</v>
       </c>
@@ -6986,10 +6941,10 @@
         <v>774</v>
       </c>
       <c r="P53" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>335</v>
       </c>
@@ -7036,10 +6991,10 @@
         <v>797</v>
       </c>
       <c r="P54" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>100</v>
       </c>
@@ -7086,10 +7041,10 @@
         <v>758</v>
       </c>
       <c r="P55" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>274</v>
       </c>
@@ -7136,10 +7091,10 @@
         <v>789</v>
       </c>
       <c r="P56" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>576</v>
       </c>
@@ -7183,16 +7138,13 @@
         <v>579</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="P57" t="s">
-        <v>1082</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>451</v>
       </c>
@@ -7236,13 +7188,13 @@
         <v>453</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="P58" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>714</v>
       </c>
@@ -7289,10 +7241,10 @@
         <v>851</v>
       </c>
       <c r="P59" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>219</v>
       </c>
@@ -7339,10 +7291,10 @@
         <v>783</v>
       </c>
       <c r="P60" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>444</v>
       </c>
@@ -7389,10 +7341,10 @@
         <v>812</v>
       </c>
       <c r="P61" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>474</v>
       </c>
@@ -7436,13 +7388,13 @@
         <v>477</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="P62" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>286</v>
       </c>
@@ -7489,10 +7441,10 @@
         <v>792</v>
       </c>
       <c r="P63" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>611</v>
       </c>
@@ -7539,10 +7491,10 @@
         <v>835</v>
       </c>
       <c r="P64" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>565</v>
       </c>
@@ -7586,13 +7538,13 @@
         <v>567</v>
       </c>
       <c r="O65" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="P65" t="s">
-        <v>1078</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>58</v>
       </c>
@@ -7636,13 +7588,13 @@
         <v>61</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="P66" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>524</v>
       </c>
@@ -7689,10 +7641,10 @@
         <v>825</v>
       </c>
       <c r="P67" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>546</v>
       </c>
@@ -7736,13 +7688,13 @@
         <v>549</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="P68" t="s">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>240</v>
       </c>
@@ -7786,13 +7738,13 @@
         <v>244</v>
       </c>
       <c r="O69" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="P69" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>492</v>
       </c>
@@ -7836,16 +7788,13 @@
         <v>494</v>
       </c>
       <c r="O70" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="P70" t="s">
-        <v>1055</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>283</v>
       </c>
@@ -7892,10 +7841,10 @@
         <v>791</v>
       </c>
       <c r="P71" t="s">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>728</v>
       </c>
@@ -7939,13 +7888,13 @@
         <v>731</v>
       </c>
       <c r="O72" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="P72" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -7992,10 +7941,10 @@
         <v>754</v>
       </c>
       <c r="P73" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>696</v>
       </c>
@@ -8042,10 +7991,10 @@
         <v>848</v>
       </c>
       <c r="P74" t="s">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>31</v>
       </c>
@@ -8092,10 +8041,10 @@
         <v>743</v>
       </c>
       <c r="P75" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>130</v>
       </c>
@@ -8139,13 +8088,13 @@
         <v>132</v>
       </c>
       <c r="O76" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="P76" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>669</v>
       </c>
@@ -8192,10 +8141,10 @@
         <v>842</v>
       </c>
       <c r="P77" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>535</v>
       </c>
@@ -8239,13 +8188,13 @@
         <v>538</v>
       </c>
       <c r="O78" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="P78" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>172</v>
       </c>
@@ -8292,10 +8241,10 @@
         <v>773</v>
       </c>
       <c r="P79" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>142</v>
       </c>
@@ -8342,10 +8291,10 @@
         <v>765</v>
       </c>
       <c r="P80" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>228</v>
       </c>
@@ -8389,13 +8338,13 @@
         <v>231</v>
       </c>
       <c r="O81" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="P81" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>602</v>
       </c>
@@ -8439,13 +8388,13 @@
         <v>605</v>
       </c>
       <c r="O82" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="P82" t="s">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>721</v>
       </c>
@@ -8492,10 +8441,10 @@
         <v>852</v>
       </c>
       <c r="P83" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>314</v>
       </c>
@@ -8539,13 +8488,13 @@
         <v>316</v>
       </c>
       <c r="O84" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="P84" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>224</v>
       </c>
@@ -8592,10 +8541,10 @@
         <v>784</v>
       </c>
       <c r="P85" t="s">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>520</v>
       </c>
@@ -8642,10 +8591,10 @@
         <v>824</v>
       </c>
       <c r="P86" t="s">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>200</v>
       </c>
@@ -8692,10 +8641,10 @@
         <v>780</v>
       </c>
       <c r="P87" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -8742,10 +8691,10 @@
         <v>747</v>
       </c>
       <c r="P88" t="s">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>599</v>
       </c>
@@ -8789,13 +8738,13 @@
         <v>601</v>
       </c>
       <c r="O89" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="P89" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>512</v>
       </c>
@@ -8842,10 +8791,10 @@
         <v>823</v>
       </c>
       <c r="P90" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>264</v>
       </c>
@@ -8889,13 +8838,13 @@
         <v>266</v>
       </c>
       <c r="O91" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="P91" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>193</v>
       </c>
@@ -8942,10 +8891,10 @@
         <v>779</v>
       </c>
       <c r="P92" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>629</v>
       </c>
@@ -8992,10 +8941,10 @@
         <v>861</v>
       </c>
       <c r="P93" t="s">
-        <v>1096</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>298</v>
       </c>
@@ -9042,10 +8991,10 @@
         <v>794</v>
       </c>
       <c r="P94" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>470</v>
       </c>
@@ -9089,16 +9038,13 @@
         <v>473</v>
       </c>
       <c r="O95" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="P95" t="s">
-        <v>1048</v>
-      </c>
-      <c r="Q95" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>332</v>
       </c>
@@ -9142,13 +9088,13 @@
         <v>334</v>
       </c>
       <c r="O96" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="P96" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>324</v>
       </c>
@@ -9192,13 +9138,13 @@
         <v>327</v>
       </c>
       <c r="O97" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="P97" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>306</v>
       </c>
@@ -9242,13 +9188,13 @@
         <v>309</v>
       </c>
       <c r="O98" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="P98" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>704</v>
       </c>
@@ -9295,13 +9241,10 @@
         <v>860</v>
       </c>
       <c r="P99" t="s">
-        <v>1118</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>328</v>
       </c>
@@ -9345,13 +9288,13 @@
         <v>331</v>
       </c>
       <c r="O100" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="P100" t="s">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>680</v>
       </c>
@@ -9395,13 +9338,13 @@
         <v>682</v>
       </c>
       <c r="O101" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="P101" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>663</v>
       </c>
@@ -9445,13 +9388,13 @@
         <v>665</v>
       </c>
       <c r="O102" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="P102" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>732</v>
       </c>
@@ -9498,10 +9441,10 @@
         <v>854</v>
       </c>
       <c r="P103" t="s">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>351</v>
       </c>
@@ -9548,10 +9491,10 @@
         <v>800</v>
       </c>
       <c r="P104" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>235</v>
       </c>
@@ -9595,13 +9538,13 @@
         <v>239</v>
       </c>
       <c r="O105" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="P105" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -9648,10 +9591,10 @@
         <v>759</v>
       </c>
       <c r="P106" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>232</v>
       </c>
@@ -9695,13 +9638,13 @@
         <v>234</v>
       </c>
       <c r="O107" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="P107" t="s">
-        <v>986</v>
-      </c>
-    </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>393</v>
       </c>
@@ -9745,13 +9688,13 @@
         <v>395</v>
       </c>
       <c r="O108" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="P108" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>162</v>
       </c>
@@ -9798,10 +9741,10 @@
         <v>770</v>
       </c>
       <c r="P109" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>355</v>
       </c>
@@ -9848,10 +9791,10 @@
         <v>801</v>
       </c>
       <c r="P110" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>666</v>
       </c>
@@ -9895,13 +9838,13 @@
         <v>668</v>
       </c>
       <c r="O111" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="P111" t="s">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>121</v>
       </c>
@@ -9948,10 +9891,10 @@
         <v>763</v>
       </c>
       <c r="P112" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>401</v>
       </c>
@@ -9995,13 +9938,13 @@
         <v>404</v>
       </c>
       <c r="O113" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="P113" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>554</v>
       </c>
@@ -10045,13 +9988,13 @@
         <v>556</v>
       </c>
       <c r="O114" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="P114" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>557</v>
       </c>
@@ -10098,10 +10041,10 @@
         <v>827</v>
       </c>
       <c r="P115" t="s">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>672</v>
       </c>
@@ -10148,10 +10091,10 @@
         <v>843</v>
       </c>
       <c r="P116" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>689</v>
       </c>
@@ -10198,10 +10141,10 @@
         <v>846</v>
       </c>
       <c r="P117" t="s">
-        <v>1114</v>
-      </c>
-    </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>675</v>
       </c>
@@ -10245,16 +10188,13 @@
         <v>679</v>
       </c>
       <c r="O118" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="P118" t="s">
-        <v>1109</v>
-      </c>
-      <c r="Q118" t="s">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>642</v>
       </c>
@@ -10298,13 +10238,13 @@
         <v>646</v>
       </c>
       <c r="O119" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="P119" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>482</v>
       </c>
@@ -10348,13 +10288,13 @@
         <v>484</v>
       </c>
       <c r="O120" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="P120" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>257</v>
       </c>
@@ -10398,13 +10338,13 @@
         <v>259</v>
       </c>
       <c r="O121" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="P121" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>36</v>
       </c>
@@ -10451,10 +10391,10 @@
         <v>744</v>
       </c>
       <c r="P122" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>459</v>
       </c>
@@ -10501,10 +10441,10 @@
         <v>815</v>
       </c>
       <c r="P123" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>216</v>
       </c>
@@ -10548,13 +10488,13 @@
         <v>218</v>
       </c>
       <c r="O124" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="P124" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>133</v>
       </c>
@@ -10598,13 +10538,13 @@
         <v>137</v>
       </c>
       <c r="O125" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="P125" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>320</v>
       </c>
@@ -10648,13 +10588,13 @@
         <v>323</v>
       </c>
       <c r="O126" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="P126" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>250</v>
       </c>
@@ -10698,13 +10638,13 @@
         <v>256</v>
       </c>
       <c r="O127" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="P127" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>425</v>
       </c>
@@ -10748,13 +10688,13 @@
         <v>428</v>
       </c>
       <c r="O128" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="P128" t="s">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>278</v>
       </c>
@@ -10801,10 +10741,10 @@
         <v>790</v>
       </c>
       <c r="P129" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>14</v>
       </c>
@@ -10851,10 +10791,10 @@
         <v>739</v>
       </c>
       <c r="P130" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>368</v>
       </c>
@@ -10898,13 +10838,13 @@
         <v>372</v>
       </c>
       <c r="O131" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="P131" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>413</v>
       </c>
@@ -10948,16 +10888,13 @@
         <v>416</v>
       </c>
       <c r="O132" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="P132" t="s">
-        <v>1031</v>
-      </c>
-      <c r="Q132" t="s">
-        <v>1032</v>
-      </c>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>539</v>
       </c>
@@ -11001,13 +10938,13 @@
         <v>542</v>
       </c>
       <c r="O133" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="P133" t="s">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>178</v>
       </c>
@@ -11054,10 +10991,10 @@
         <v>775</v>
       </c>
       <c r="P134" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>169</v>
       </c>
@@ -11104,10 +11041,10 @@
         <v>772</v>
       </c>
       <c r="P135" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>417</v>
       </c>
@@ -11151,13 +11088,13 @@
         <v>420</v>
       </c>
       <c r="O136" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="P136" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>364</v>
       </c>
@@ -11204,10 +11141,10 @@
         <v>803</v>
       </c>
       <c r="P137" t="s">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>40</v>
       </c>
@@ -11254,10 +11191,10 @@
         <v>745</v>
       </c>
       <c r="P138" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>343</v>
       </c>
@@ -11301,13 +11238,13 @@
         <v>346</v>
       </c>
       <c r="O139" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="P139" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>647</v>
       </c>
@@ -11354,10 +11291,10 @@
         <v>839</v>
       </c>
       <c r="P140" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>421</v>
       </c>
@@ -11401,16 +11338,13 @@
         <v>424</v>
       </c>
       <c r="O141" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="P141" t="s">
-        <v>1034</v>
-      </c>
-      <c r="Q141" t="s">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>159</v>
       </c>
@@ -11457,10 +11391,10 @@
         <v>769</v>
       </c>
       <c r="P142" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>618</v>
       </c>
@@ -11507,10 +11441,10 @@
         <v>837</v>
       </c>
       <c r="P143" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>686</v>
       </c>
@@ -11557,10 +11491,10 @@
         <v>845</v>
       </c>
       <c r="P144" t="s">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>508</v>
       </c>
@@ -11607,13 +11541,10 @@
         <v>822</v>
       </c>
       <c r="P145" t="s">
-        <v>1061</v>
-      </c>
-      <c r="Q145" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>204</v>
       </c>
@@ -11660,10 +11591,10 @@
         <v>781</v>
       </c>
       <c r="P146" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>499</v>
       </c>
@@ -11707,16 +11638,13 @@
         <v>503</v>
       </c>
       <c r="O147" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="P147" t="s">
-        <v>1058</v>
-      </c>
-      <c r="Q147" t="s">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>495</v>
       </c>
@@ -11763,10 +11691,10 @@
         <v>820</v>
       </c>
       <c r="P148" t="s">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>708</v>
       </c>
@@ -11813,13 +11741,10 @@
         <v>862</v>
       </c>
       <c r="P149" t="s">
-        <v>1120</v>
-      </c>
-      <c r="Q149" t="s">
-        <v>1121</v>
-      </c>
-    </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>651</v>
       </c>
@@ -11863,13 +11788,13 @@
         <v>654</v>
       </c>
       <c r="O150" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="P150" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>531</v>
       </c>
@@ -11913,13 +11838,13 @@
         <v>534</v>
       </c>
       <c r="O151" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="P151" t="s">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>290</v>
       </c>
@@ -11966,10 +11891,10 @@
         <v>793</v>
       </c>
       <c r="P152" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>588</v>
       </c>
@@ -12016,10 +11941,10 @@
         <v>832</v>
       </c>
       <c r="P153" t="s">
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>154</v>
       </c>
@@ -12066,10 +11991,10 @@
         <v>768</v>
       </c>
       <c r="P154" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>516</v>
       </c>
@@ -12113,13 +12038,13 @@
         <v>519</v>
       </c>
       <c r="O155" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="P155" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>53</v>
       </c>
@@ -12166,10 +12091,10 @@
         <v>748</v>
       </c>
       <c r="P156" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>440</v>
       </c>
@@ -12216,13 +12141,10 @@
         <v>857</v>
       </c>
       <c r="P157" t="s">
-        <v>1038</v>
-      </c>
-      <c r="Q157" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>88</v>
       </c>
@@ -12269,10 +12191,10 @@
         <v>755</v>
       </c>
       <c r="P158" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>96</v>
       </c>
@@ -12319,10 +12241,10 @@
         <v>757</v>
       </c>
       <c r="P159" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>592</v>
       </c>
@@ -12366,13 +12288,13 @@
         <v>595</v>
       </c>
       <c r="O160" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="P160" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>596</v>
       </c>
@@ -12419,10 +12341,10 @@
         <v>833</v>
       </c>
       <c r="P161" t="s">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>717</v>
       </c>
@@ -12466,16 +12388,13 @@
         <v>720</v>
       </c>
       <c r="O162" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="P162" t="s">
-        <v>1123</v>
-      </c>
-      <c r="Q162" t="s">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>693</v>
       </c>
@@ -12522,10 +12441,10 @@
         <v>847</v>
       </c>
       <c r="P163" t="s">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>188</v>
       </c>
@@ -12572,10 +12491,10 @@
         <v>778</v>
       </c>
       <c r="P164" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>302</v>
       </c>
@@ -12619,13 +12538,13 @@
         <v>305</v>
       </c>
       <c r="O165" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="P165" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>23</v>
       </c>
@@ -12672,10 +12591,10 @@
         <v>741</v>
       </c>
       <c r="P166" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>117</v>
       </c>
@@ -12722,10 +12641,10 @@
         <v>762</v>
       </c>
       <c r="P167" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>108</v>
       </c>
@@ -12772,10 +12691,10 @@
         <v>760</v>
       </c>
       <c r="P168" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>632</v>
       </c>
@@ -12822,10 +12741,10 @@
         <v>838</v>
       </c>
       <c r="P169" t="s">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>735</v>
       </c>
@@ -12872,10 +12791,10 @@
         <v>855</v>
       </c>
       <c r="P170" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>70</v>
       </c>
@@ -12922,10 +12841,10 @@
         <v>751</v>
       </c>
       <c r="P171" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>347</v>
       </c>
@@ -12972,10 +12891,10 @@
         <v>799</v>
       </c>
       <c r="P172" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>19</v>
       </c>
@@ -13022,10 +12941,10 @@
         <v>740</v>
       </c>
       <c r="P173" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>181</v>
       </c>
@@ -13072,10 +12991,10 @@
         <v>776</v>
       </c>
       <c r="P174" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>625</v>
       </c>
@@ -13122,10 +13041,10 @@
         <v>859</v>
       </c>
       <c r="P175" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>622</v>
       </c>
@@ -13172,10 +13091,10 @@
         <v>781</v>
       </c>
       <c r="P176" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>339</v>
       </c>
@@ -13222,10 +13141,10 @@
         <v>798</v>
       </c>
       <c r="P177" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>489</v>
       </c>
@@ -13272,10 +13191,10 @@
         <v>819</v>
       </c>
       <c r="P178" t="s">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>485</v>
       </c>
@@ -13322,10 +13241,10 @@
         <v>818</v>
       </c>
       <c r="P179" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>658</v>
       </c>
@@ -13372,10 +13291,10 @@
         <v>841</v>
       </c>
       <c r="P180" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>85</v>
       </c>
@@ -13419,13 +13338,13 @@
         <v>87</v>
       </c>
       <c r="O181" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="P181" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>197</v>
       </c>
@@ -13469,13 +13388,13 @@
         <v>199</v>
       </c>
       <c r="O182" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="P182" t="s">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>550</v>
       </c>
@@ -13519,16 +13438,13 @@
         <v>553</v>
       </c>
       <c r="O183" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="P183" t="s">
-        <v>1073</v>
-      </c>
-      <c r="Q183" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>448</v>
       </c>
@@ -13575,10 +13491,10 @@
         <v>813</v>
       </c>
       <c r="P184" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>580</v>
       </c>
@@ -13625,10 +13541,10 @@
         <v>830</v>
       </c>
       <c r="P185" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>700</v>
       </c>
@@ -13675,11 +13591,10 @@
         <v>849</v>
       </c>
       <c r="P186" t="s">
-        <v>1117</v>
-      </c>
-      <c r="R186" s="8"/>
-    </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>405</v>
       </c>
@@ -13726,10 +13641,10 @@
         <v>809</v>
       </c>
       <c r="P187" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>429</v>
       </c>
@@ -13773,16 +13688,13 @@
         <v>432</v>
       </c>
       <c r="O188" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="P188" t="s">
-        <v>1130</v>
-      </c>
-      <c r="Q188" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>381</v>
       </c>
@@ -13826,37 +13738,357 @@
         <v>384</v>
       </c>
       <c r="O189" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="P189" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K190" s="1"/>
       <c r="L190" s="1"/>
-    </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P190" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L191" s="1"/>
-    </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P191" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K192" s="1"/>
       <c r="L192" s="1"/>
-    </row>
-    <row r="193" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="P192" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="193" spans="5:16" x14ac:dyDescent="0.25">
       <c r="K193" s="1"/>
-    </row>
-    <row r="194" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="P193" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="194" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E194" s="1"/>
+      <c r="P194" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="195" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P195" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="196" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P196" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="197" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P197" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="198" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P198" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="199" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P199" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="200" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P200" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="201" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P201" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="202" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P202" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="203" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P203" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="204" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P204" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="205" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P205" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="206" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P206" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="207" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P207" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="208" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="P208" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="209" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P209" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="210" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P210" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="211" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P211" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="212" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P212" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="213" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P213" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="214" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P214" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="215" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P215" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="216" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P216" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="217" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P217" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="218" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P218" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="219" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P219" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="220" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P220" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="221" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P221" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="222" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P222" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="223" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P223" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="224" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P224" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="225" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P225" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="226" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P226" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="227" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P227" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="228" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P228" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="229" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P229" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="230" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P230" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="231" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P231" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="232" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P232" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="233" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P233" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="234" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P234" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="235" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P235" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="236" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P236" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="237" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P237" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="238" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P238" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="239" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P239" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="240" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P240" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="241" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P241" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="242" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P242" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="243" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P243" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="244" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P244" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="245" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P245" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="246" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P246" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="247" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P247" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="248" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P248" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="249" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P249" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="250" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P250" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="251" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P251" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="252" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P252" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="253" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P253" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="254" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P254" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="255" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P255" t="s">
+        <v>1117</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R297" xr:uid="{F31E04C9-FD1B-4371-89BD-EFAF6083FB56}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R297">
+  <autoFilter ref="A1:O297" xr:uid="{F31E04C9-FD1B-4371-89BD-EFAF6083FB56}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O297">
       <sortCondition ref="A1:A297"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="27" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="24" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13876,10 +14108,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13887,7 +14119,7 @@
         <v>197</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13895,7 +14127,7 @@
         <v>232</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13903,7 +14135,7 @@
         <v>240</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13911,7 +14143,7 @@
         <v>257</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13919,7 +14151,7 @@
         <v>294</v>
       </c>
       <c r="C6" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13927,7 +14159,7 @@
         <v>306</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13935,7 +14167,7 @@
         <v>332</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13943,7 +14175,7 @@
         <v>417</v>
       </c>
       <c r="C10" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13951,7 +14183,7 @@
         <v>516</v>
       </c>
       <c r="C12" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13959,7 +14191,7 @@
         <v>531</v>
       </c>
       <c r="C13" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13967,7 +14199,7 @@
         <v>638</v>
       </c>
       <c r="C14" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13975,7 +14207,7 @@
         <v>728</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
@@ -13983,7 +14215,7 @@
     </row>
     <row r="17" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
@@ -13991,7 +14223,7 @@
         <v>425</v>
       </c>
       <c r="C18" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
@@ -13999,7 +14231,7 @@
         <v>554</v>
       </c>
       <c r="C19" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
@@ -14007,7 +14239,7 @@
         <v>602</v>
       </c>
       <c r="C20" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
@@ -14015,7 +14247,7 @@
         <v>663</v>
       </c>
       <c r="C21" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
@@ -14023,7 +14255,7 @@
         <v>680</v>
       </c>
       <c r="C22" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
@@ -14031,7 +14263,7 @@
     </row>
     <row r="24" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>

</xml_diff>